<commit_message>
Updating RTM by connecting Test cases with last version of SRS
</commit_message>
<xml_diff>
--- a/Workspace/Testing/ACS_TC.xlsx
+++ b/Workspace/Testing/ACS_TC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -119,30 +119,9 @@
     <t>TC_2.2</t>
   </si>
   <si>
-    <t>Check when we press ON button again when the conditioner is already on</t>
-  </si>
-  <si>
-    <t>Press ON button after 5 seconds from press ON button first time</t>
-  </si>
-  <si>
-    <t>1. Make a short voice of the ON/OFF buttons without doing anything else</t>
-  </si>
-  <si>
     <t>TC_2.3</t>
   </si>
   <si>
-    <t>Check when we press OFF button again when the conditioner is already off</t>
-  </si>
-  <si>
-    <t>The conditioner should be turned off</t>
-  </si>
-  <si>
-    <t>Press OFF button again after 5 seconds</t>
-  </si>
-  <si>
-    <t>1. Make a short voice of the ON/OFF buttons  without doing anythimg else</t>
-  </si>
-  <si>
     <t>TC_2.4</t>
   </si>
   <si>
@@ -152,12 +131,6 @@
     <t>Does not accept any request from any button until 5 seconds ends</t>
   </si>
   <si>
-    <t>TC_2.5</t>
-  </si>
-  <si>
-    <t>Check when we press any button within 5 seconds after press OFFbutton</t>
-  </si>
-  <si>
     <t>press any button within 5 seconds after pressing OFF button</t>
   </si>
   <si>
@@ -168,14 +141,6 @@
   </si>
   <si>
     <t>Check when we press up button while temp degree was 32</t>
-  </si>
-  <si>
-    <t>The conditioner should be turned on
-The mode button should be pressed once and the cursor should be stopped in the temp degree line
-The temp degree should be 32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Press UP button to increase the temp degree </t>
   </si>
   <si>
     <t>1. The button should make a voice of the UP/DOWN button
@@ -188,14 +153,6 @@
     <t>Check when we press down button while temp degree was 16</t>
   </si>
   <si>
-    <t>The conditioner should be turned on
-The mode button should be pressed once and the cursor should be stopped in the temp degree line
-The temp degree should be 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Press DOWN button to decrease the temp degree </t>
-  </si>
-  <si>
     <t>1. The button should make a voice of the UP/DOWN button
 2. The temp degree should not decrease and does not change and should still 16</t>
   </si>
@@ -206,14 +163,6 @@
     <t>Check when we press up button while fan speed was high</t>
   </si>
   <si>
-    <t>"The conditioner should be turned on
-The mode button should be pressed twice and the cursor should be stopped in the fan speed line
-The fan speed should be high</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Press UP button to increase the fan speed </t>
-  </si>
-  <si>
     <t>1. The button should make a voice of the UP/DOWN button
 2. The fan level should not increase and does not change and should still high</t>
   </si>
@@ -224,14 +173,6 @@
     <t>Check when we press down button while fan level was low</t>
   </si>
   <si>
-    <t>"The conditioner should be turned on
-The mode button should be pressed twice and the cursor should be stopped in the fan speed line
-The fan speed should be low</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Press DOWN button to decrease the fan speed </t>
-  </si>
-  <si>
     <t>1. The button should make a voice of the UP/DOWN button
 2. The fan level should not decrease and does not change and should still low</t>
   </si>
@@ -242,14 +183,6 @@
     <t>Check when we long press UP button</t>
   </si>
   <si>
-    <t xml:space="preserve">The conditioner should be turned on
-The mode button should be pressed once and the cursor should be stopped in the temp degree line
-</t>
-  </si>
-  <si>
-    <t>long press UP button</t>
-  </si>
-  <si>
     <t>1. The button should make a voice of the UP/DOWN button
 2. The temp degree should increase 1 degree</t>
   </si>
@@ -260,9 +193,6 @@
     <t>Check when we long press DOWN button</t>
   </si>
   <si>
-    <t>long press DOWN button</t>
-  </si>
-  <si>
     <t>1. The button should make a voice of the UP/DOWN button
 2. The temp degree should decrease 1 degree</t>
   </si>
@@ -273,12 +203,6 @@
     <t>Check when we press UP/Down button in the display screen</t>
   </si>
   <si>
-    <t>The conditioner should be turned on and the display screen should opend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Press UP/DOWN button </t>
-  </si>
-  <si>
     <t xml:space="preserve">It should not do anything </t>
   </si>
   <si>
@@ -311,9 +235,6 @@
   </si>
   <si>
     <t>TC_1.9</t>
-  </si>
-  <si>
-    <t>TC_2.6</t>
   </si>
   <si>
     <t>TC_3.7</t>
@@ -437,13 +358,54 @@
   </si>
   <si>
     <t>Check when we press any button within 5 seconds after press ON/OFF button</t>
+  </si>
+  <si>
+    <t>Check when we press any button within 5 seconds after press ON/OFFbutton</t>
+  </si>
+  <si>
+    <t>1. Press ON/OFF button to open the air conditioner
+2. After 5 seconds press mode button to go to the menu screen to change the temp degree
+3. Long press up button to increase the temp degree</t>
+  </si>
+  <si>
+    <t>The fan speed must be low</t>
+  </si>
+  <si>
+    <t>The fan speed must be high</t>
+  </si>
+  <si>
+    <t>The temp degree must be 16</t>
+  </si>
+  <si>
+    <t>The temp degree must be 32</t>
+  </si>
+  <si>
+    <t>1. Press ON/OFF button to open the air conditioner
+2. After 5 seconds press mode button to go to the menu screen to change the temp degree
+3. Long press up button to decrease the temp degree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Press ON/OFF button to open the air conditioner
+2. After 5 seconds ress UP/DOWN button </t>
+  </si>
+  <si>
+    <t>Project Name:</t>
+  </si>
+  <si>
+    <t>Digital Air Conditioner Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Version Number:</t>
+  </si>
+  <si>
+    <t>Version 3.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -454,25 +416,30 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -491,6 +458,35 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -507,12 +503,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFEAD1DC"/>
         <bgColor rgb="FFEAD1DC"/>
       </patternFill>
@@ -523,8 +513,14 @@
         <bgColor rgb="FFA4C2F4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -569,11 +565,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -596,52 +601,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -667,7 +650,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -683,6 +665,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -966,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C30"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -981,103 +1002,95 @@
     <col min="8" max="8" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:27" s="32" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+    </row>
+    <row r="2" spans="1:27" s="32" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+    </row>
+    <row r="3" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-    </row>
-    <row r="2" spans="1:27" s="16" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-    </row>
-    <row r="3" spans="1:27" ht="60" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1098,64 +1111,58 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
     </row>
-    <row r="4" spans="1:27" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-    </row>
-    <row r="5" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+    <row r="4" spans="1:27" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+    </row>
+    <row r="5" spans="1:27" ht="60" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -1176,25 +1183,25 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
     </row>
-    <row r="6" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+    <row r="6" spans="1:27" ht="90" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="42"/>
+      <c r="C6" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1216,22 +1223,24 @@
       <c r="AA6" s="5"/>
     </row>
     <row r="7" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
+      <c r="A7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="42"/>
+      <c r="C7" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -1253,24 +1262,24 @@
       <c r="AA7" s="5"/>
     </row>
     <row r="8" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="A8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -1292,22 +1301,22 @@
       <c r="AA8" s="5"/>
     </row>
     <row r="9" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="A9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -1328,23 +1337,25 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
     </row>
-    <row r="10" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+    <row r="10" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="42"/>
+      <c r="C10" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1365,23 +1376,23 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
     </row>
-    <row r="11" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
+    <row r="11" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -1402,15 +1413,23 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
     </row>
-    <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+    <row r="12" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="42"/>
+      <c r="C12" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -1431,19 +1450,23 @@
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
     </row>
-    <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+    <row r="13" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="42"/>
+      <c r="C13" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -1464,27 +1487,15 @@
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
     </row>
-    <row r="14" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -1505,23 +1516,17 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
     </row>
-    <row r="15" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>28</v>
-      </c>
+    <row r="15" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1544,22 +1549,24 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
     </row>
-    <row r="16" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>25</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1583,22 +1590,22 @@
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
     </row>
-    <row r="17" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1624,20 +1631,20 @@
     </row>
     <row r="18" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -1663,20 +1670,20 @@
     </row>
     <row r="19" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1701,12 +1708,12 @@
       <c r="AA19" s="5"/>
     </row>
     <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="5"/>
@@ -1730,13 +1737,13 @@
       <c r="AA20" s="5"/>
     </row>
     <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="19"/>
+      <c r="A21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="39"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1762,27 +1769,27 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
     </row>
-    <row r="22" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+    <row r="22" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -1803,25 +1810,25 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
     </row>
-    <row r="23" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
+    <row r="23" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="42"/>
+      <c r="C23" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -1842,25 +1849,25 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
     </row>
-    <row r="24" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
+    <row r="24" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="42"/>
+      <c r="C24" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -1881,25 +1888,25 @@
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
-    <row r="25" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
+    <row r="25" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="42"/>
+      <c r="C25" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -1920,25 +1927,25 @@
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
     </row>
-    <row r="26" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
+    <row r="26" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="42"/>
+      <c r="C26" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -1959,25 +1966,25 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
     </row>
-    <row r="27" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
+    <row r="27" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="42"/>
+      <c r="C27" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -1999,24 +2006,22 @@
       <c r="AA27" s="5"/>
     </row>
     <row r="28" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="42"/>
+      <c r="C28" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -2067,13 +2072,13 @@
       <c r="AA29" s="5"/>
     </row>
     <row r="30" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="19"/>
+      <c r="A30" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="39"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
@@ -2100,26 +2105,26 @@
       <c r="AA30" s="5"/>
     </row>
     <row r="31" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="25" t="s">
+      <c r="A31" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
+      <c r="E31" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -2170,25 +2175,25 @@
       <c r="AA32" s="5"/>
     </row>
     <row r="33" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="25" t="s">
+      <c r="A33" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" s="28"/>
+      <c r="E33" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="20"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -2211,76 +2216,76 @@
       <c r="AA33" s="5"/>
     </row>
     <row r="34" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="28"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="38"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="29"/>
     </row>
     <row r="35" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="28"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="38"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="29"/>
     </row>
     <row r="36" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="28"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="38"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="29"/>
     </row>
     <row r="37" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="28"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="38"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="29"/>
     </row>
     <row r="38" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="28"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="38"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="29"/>
     </row>
     <row r="39" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="28"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="38"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="29"/>
     </row>
     <row r="40" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="28"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="38"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="29"/>
     </row>
     <row r="41" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="28"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="38"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="29"/>
     </row>
     <row r="42" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
@@ -9987,15 +9992,20 @@
       <c r="F1004" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B2:C2"/>
+  <mergeCells count="11">
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B22:B28"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reply on Ramdan comment changing tc 3.1
</commit_message>
<xml_diff>
--- a/Workspace/Testing/ACS_TC.xlsx
+++ b/Workspace/Testing/ACS_TC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI intake 38\26- Project Management with Embeded\Air-Conditioner-Screen-Team-4\Workspace\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Air-Conditioner-Screen-Team-4\Workspace\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -180,9 +180,6 @@
     <t>TC_3.4</t>
   </si>
   <si>
-    <t>Check when we long press UP button</t>
-  </si>
-  <si>
     <t>1. The button should make a voice of the UP/DOWN button
 2. The temp degree should increase 1 degree</t>
   </si>
@@ -399,6 +396,9 @@
   </si>
   <si>
     <t>Version 3.0</t>
+  </si>
+  <si>
+    <t>Checking   long press on UP button</t>
   </si>
 </sst>
 </file>
@@ -670,6 +670,23 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -686,23 +703,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1003,18 +1003,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="32" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
       <c r="I1" s="31"/>
       <c r="J1" s="31"/>
       <c r="K1" s="31"/>
@@ -1035,18 +1035,18 @@
       <c r="Z1" s="31"/>
     </row>
     <row r="2" spans="1:27" s="32" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
@@ -1113,12 +1113,12 @@
     </row>
     <row r="4" spans="1:27" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="39"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
@@ -1148,15 +1148,15 @@
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>9</v>
@@ -1187,18 +1187,18 @@
       <c r="A6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="42"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="F6" s="26" t="s">
         <v>73</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>74</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
@@ -1226,15 +1226,15 @@
       <c r="A7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="42"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>75</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>76</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>12</v>
@@ -1265,15 +1265,15 @@
       <c r="A8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="42"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>77</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>78</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>14</v>
@@ -1304,16 +1304,16 @@
       <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="42"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>81</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -1341,15 +1341,15 @@
       <c r="A10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="42"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E10" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>84</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>17</v>
@@ -1380,13 +1380,13 @@
       <c r="A11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="42"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>19</v>
@@ -1417,16 +1417,16 @@
       <c r="A12" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="42"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -1452,15 +1452,15 @@
     </row>
     <row r="13" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="42"/>
+        <v>65</v>
+      </c>
+      <c r="B13" s="36"/>
       <c r="C13" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>22</v>
@@ -1520,10 +1520,10 @@
       <c r="A15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="39"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
@@ -1553,17 +1553,17 @@
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="37" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>96</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>25</v>
@@ -1594,15 +1594,15 @@
       <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="39"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="E17" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>99</v>
       </c>
       <c r="F17" s="21" t="s">
         <v>28</v>
@@ -1633,12 +1633,12 @@
       <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="39"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>32</v>
@@ -1672,12 +1672,12 @@
       <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="39"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" s="28" t="s">
         <v>34</v>
@@ -1740,10 +1740,10 @@
       <c r="A21" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1773,17 +1773,17 @@
       <c r="A22" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="35" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>38</v>
@@ -1814,15 +1814,15 @@
       <c r="A23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="42"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="17" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>41</v>
@@ -1853,15 +1853,15 @@
       <c r="A24" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="42"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="17" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>44</v>
@@ -1892,15 +1892,15 @@
       <c r="A25" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="42"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="17" t="s">
         <v>46</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" s="17" t="s">
         <v>47</v>
@@ -1929,20 +1929,20 @@
     </row>
     <row r="26" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="42"/>
+        <v>50</v>
+      </c>
+      <c r="B26" s="36"/>
       <c r="C26" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>50</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -1968,20 +1968,20 @@
     </row>
     <row r="27" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="42"/>
+        <v>53</v>
+      </c>
+      <c r="B27" s="36"/>
       <c r="C27" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>53</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -2007,18 +2007,18 @@
     </row>
     <row r="28" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="42"/>
+        <v>66</v>
+      </c>
+      <c r="B28" s="36"/>
       <c r="C28" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -2073,12 +2073,12 @@
     </row>
     <row r="30" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="39"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
@@ -2106,22 +2106,22 @@
     </row>
     <row r="31" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>61</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
@@ -2176,22 +2176,22 @@
     </row>
     <row r="33" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="C33" s="28" t="s">
         <v>63</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>64</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="5"/>
@@ -9993,17 +9993,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B5:B13"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="B22:B28"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>